<commit_message>
STAR MEM to KATL 26L
</commit_message>
<xml_diff>
--- a/trajectory/management/commands/SidStar/STAR-KATL-MEM-26L.xlsx
+++ b/trajectory/management/commands/SidStar/STAR-KATL-MEM-26L.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\git\flight-profile\trajectory\management\commands\SidStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC144F28-852A-4199-B1A8-7E9B9ADF7B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F2D751-33EC-400F-8E30-15936AC89A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E599D276-CC0B-4999-86A2-09540BAD0A64}"/>
+    <workbookView xWindow="4470" yWindow="1910" windowWidth="19200" windowHeight="11170" xr2:uid="{E599D276-CC0B-4999-86A2-09540BAD0A64}"/>
   </bookViews>
   <sheets>
-    <sheet name="Waypoints" sheetId="1" r:id="rId1"/>
+    <sheet name="WayPoints" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>order</t>
   </si>
@@ -65,21 +65,12 @@
     <t>MEMPHIS</t>
   </si>
   <si>
-    <t>W086°50'43.37"</t>
-  </si>
-  <si>
-    <t>HERKO</t>
-  </si>
-  <si>
     <t>ALABAMA</t>
   </si>
   <si>
     <t>CALCO</t>
   </si>
   <si>
-    <t>N33°04'08.67"</t>
-  </si>
-  <si>
     <t>N34°20'42.91"</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>DEVAC</t>
   </si>
   <si>
-    <t>87-26-6.6 W</t>
-  </si>
-  <si>
     <t>N34°37'05.09"</t>
   </si>
   <si>
@@ -99,6 +87,30 @@
   </si>
   <si>
     <t>W089°58'59.55"</t>
+  </si>
+  <si>
+    <t>KATL/26L</t>
+  </si>
+  <si>
+    <t>obtained from runways data</t>
+  </si>
+  <si>
+    <t>ATLANTA</t>
+  </si>
+  <si>
+    <t>W087°26'06.06"</t>
+  </si>
+  <si>
+    <t>ERLIN</t>
+  </si>
+  <si>
+    <t>N34°05'13.95"</t>
+  </si>
+  <si>
+    <t>W085°01'18.94"</t>
+  </si>
+  <si>
+    <t>GEORGIA</t>
   </si>
 </sst>
 </file>
@@ -450,16 +462,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3E1F7A-8251-4D41-A445-513320E03FDC}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.6328125" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -492,10 +505,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -509,19 +522,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -529,19 +542,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -549,19 +562,39 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>